<commit_message>
docs: update api settings
</commit_message>
<xml_diff>
--- a/docs/api-setting.xlsx
+++ b/docs/api-setting.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="161">
   <si>
     <t>API</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -664,6 +664,10 @@
   </si>
   <si>
     <t>description, createdTimestamp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>account, email, name, password, introduction</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1101,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.2" x14ac:dyDescent="0.3"/>
@@ -1361,6 +1365,9 @@
       </c>
       <c r="D13" s="2" t="s">
         <v>49</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>160</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
feat: add filter features to /api/admin/users
</commit_message>
<xml_diff>
--- a/docs/api-setting.xlsx
+++ b/docs/api-setting.xlsx
@@ -571,103 +571,103 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>關聯 user、replies、likes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>關聯 user、replies、likes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>關聯 user</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>key: followersCount、followingsCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>追蹤相關</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>取得使用者回覆過的所有貼文</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>followships</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>replies</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>功能面：點選顯示更多使用者，要更新使用者數據，開設參數 currentIndex、acculatedNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/admin/users</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/admin/tweets</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>貼文數量越多的靠前、key: tweetsCount、followingsCount、followersCount、likesCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>取得使用者喜歡的貼文</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>key: repliesCount、likesCount、isLiked</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>key: repliesCount、likesCount、isLiked</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/tweets/:tid/like</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>body</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>email, password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>account, name, email, password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">email, password </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>followingId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>comment, createdTimestamp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>description, createdTimestamp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>account, email, name, password, introduction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>/users</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>關聯 user、replies、likes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>關聯 user、replies、likes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>關聯 user</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>key: followersCount、followingsCount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>追蹤相關</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>取得使用者回覆過的所有貼文</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>followships</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>replies</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>功能面：點選顯示更多使用者，要更新使用者數據，開設參數 currentIndex、acculatedNum</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/admin/users</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/admin/tweets</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>貼文數量越多的靠前、key: tweetsCount、followingsCount、followersCount、likesCount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>取得使用者喜歡的貼文</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>key: repliesCount、likesCount、isLiked</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>key: repliesCount、likesCount、isLiked</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/tweets/:tid/like</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>body</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>email, password</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>account, name, email, password</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">email, password </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>followingId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>comment, createdTimestamp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>description, createdTimestamp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>account, email, name, password, introduction</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1105,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.2" x14ac:dyDescent="0.3"/>
@@ -1132,7 +1132,7 @@
         <v>33</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>50</v>
@@ -1155,7 +1155,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>35</v>
@@ -1185,7 +1185,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>38</v>
@@ -1197,7 +1197,7 @@
         <v>4</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -1212,7 +1212,7 @@
         <v>39</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>52</v>
@@ -1251,7 +1251,7 @@
         <v>40</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>53</v>
@@ -1269,7 +1269,7 @@
         <v>41</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>54</v>
@@ -1283,7 +1283,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>17</v>
@@ -1301,7 +1301,7 @@
         <v>46</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -1346,7 +1346,7 @@
         <v>25</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>61</v>
@@ -1367,13 +1367,13 @@
         <v>49</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>58</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1421,10 +1421,10 @@
         <v>127</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>128</v>
@@ -1432,7 +1432,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>120</v>
@@ -1444,7 +1444,7 @@
         <v>122</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1459,10 +1459,10 @@
         <v>119</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>130</v>
@@ -1485,10 +1485,10 @@
         <v>64</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>19</v>
@@ -1509,10 +1509,10 @@
         <v>69</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1543,7 +1543,7 @@
         <v>71</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>64</v>
@@ -1561,7 +1561,7 @@
         <v>21</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>73</v>
@@ -1578,7 +1578,7 @@
         <v>132</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -1586,7 +1586,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>133</v>

</xml_diff>